<commit_message>
book,author - list,detail page
</commit_message>
<xml_diff>
--- a/Django/locallibrary/log.xlsx
+++ b/Django/locallibrary/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AI\pythonProject\venv\develop\seok-young\Django\locallibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13C34893-23AF-4A28-BCD9-E26338EF4EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BF5EBD-5408-4007-A900-D61239C8E6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{06DAE240-7637-4392-AC71-5B9B1262A298}"/>
+    <workbookView xWindow="11340" yWindow="0" windowWidth="11700" windowHeight="12360" xr2:uid="{06DAE240-7637-4392-AC71-5B9B1262A298}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>네이버 API발급</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,6 +55,66 @@
   </si>
   <si>
     <t>locallibrary 모델 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국립중앙도서관 API 발급</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홈페이지 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>책 디테일페이지 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>책 리스트페이지 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작가 리스트페이지 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작가 디테일페이지 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세션 설정 및 저장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자 계정 생성 및 권한설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>책대여갱신프로세스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>폼 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unit testing 자동화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국립중앙도서관 api 자료 다운로드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오라클 DB에 저장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오라클 - 로컬라이브러리 서버 연결</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -442,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3D4221-C754-40FB-9E43-9BA0D2184112}">
-  <dimension ref="A2:B7"/>
+  <dimension ref="A2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -493,6 +553,85 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" s="1">
+        <v>45530</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" s="1">
+        <v>45531</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>